<commit_message>
feat: 04_03 überarbeitet inklusive Excel Änderung + references erweitert
</commit_message>
<xml_diff>
--- a/Excel/04_03_Matching_Framework.xlsx
+++ b/Excel/04_03_Matching_Framework.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bosch-my.sharepoint.com/personal/nnr3fe_bosch_com/Documents/PersonalDrive/HTWG/BA/LaTex/Thesis/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilsarnold/Documents/WIN-Studium/7. Semester/BA/Thesis/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="8_{F3ECA3D2-32AC-4160-8B23-5AFCB2956E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AAE2120-A746-40F4-BE24-D7F32A838880}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D0E63E-EBA2-4C49-ACFE-9EA71A4B6026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EB5A32BC-5E12-4407-AAFD-77198812C495}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="17380" xr2:uid="{EB5A32BC-5E12-4407-AAFD-77198812C495}"/>
   </bookViews>
   <sheets>
     <sheet name="4_3_1" sheetId="1" r:id="rId1"/>
@@ -202,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -211,9 +211,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -553,15 +550,15 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="41.26953125" customWidth="1"/>
+    <col min="1" max="6" width="41.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -581,7 +578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -597,11 +594,11 @@
       <c r="E2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -617,11 +614,11 @@
       <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -637,11 +634,11 @@
       <c r="E4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -657,11 +654,11 @@
       <c r="E5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -677,11 +674,12 @@
       <c r="E6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>